<commit_message>
Upd Marking and Chn
</commit_message>
<xml_diff>
--- a/Surat Jalan/AIR/Surat Jalan W99-WJY-AIR 4 Koli.xlsx
+++ b/Surat Jalan/AIR/Surat Jalan W99-WJY-AIR 4 Koli.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patrick Jonathan\Documents\Patrick Jonathan\CARGO\Cargo Work\Surat Jalan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patrick Jonathan\Documents\Patrick Jonathan\CARGO\Cargo Work\Surat Jalan\AIR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C75B12B-3655-4E74-B7E9-7EBEC2B8AD8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8E95A44-6E28-4914-9D82-DDF5A622E167}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="33">
   <si>
     <t>SURAT JALAN</t>
   </si>
@@ -127,10 +127,13 @@
     <t>Telepon</t>
   </si>
   <si>
-    <t>W99-WJY-AIR</t>
-  </si>
-  <si>
-    <t>Aksesoris</t>
+    <t>279-W99-WJY-AIR</t>
+  </si>
+  <si>
+    <t>250215W99-WJY</t>
+  </si>
+  <si>
+    <t>A0034365  Aksesoris</t>
   </si>
 </sst>
 </file>
@@ -524,7 +527,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -534,10 +536,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -552,7 +551,11 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -873,7 +876,7 @@
   <dimension ref="B1:P54"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12:O12"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -917,7 +920,9 @@
       <c r="B2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="15"/>
+      <c r="C2" s="15" t="s">
+        <v>31</v>
+      </c>
       <c r="D2" s="15"/>
       <c r="E2" s="15"/>
       <c r="K2" t="s">
@@ -926,16 +931,16 @@
       <c r="L2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="M2" s="64"/>
-      <c r="N2" s="65"/>
-      <c r="O2" s="65"/>
-      <c r="P2" s="65"/>
+      <c r="M2" s="62"/>
+      <c r="N2" s="63"/>
+      <c r="O2" s="63"/>
+      <c r="P2" s="63"/>
     </row>
     <row r="3" spans="2:16" ht="15.75" customHeight="1">
-      <c r="B3" s="56" t="s">
+      <c r="B3" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="56"/>
+      <c r="C3" s="64"/>
       <c r="D3" s="24"/>
       <c r="E3" s="19"/>
       <c r="K3" t="s">
@@ -944,18 +949,18 @@
       <c r="L3" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="M3" s="64"/>
-      <c r="N3" s="65"/>
-      <c r="O3" s="65"/>
-      <c r="P3" s="65"/>
+      <c r="M3" s="62"/>
+      <c r="N3" s="63"/>
+      <c r="O3" s="63"/>
+      <c r="P3" s="63"/>
     </row>
     <row r="4" spans="2:16" ht="15.75" customHeight="1">
       <c r="F4" s="16"/>
       <c r="L4" s="17"/>
-      <c r="M4" s="65"/>
-      <c r="N4" s="65"/>
-      <c r="O4" s="65"/>
-      <c r="P4" s="65"/>
+      <c r="M4" s="63"/>
+      <c r="N4" s="63"/>
+      <c r="O4" s="63"/>
+      <c r="P4" s="63"/>
     </row>
     <row r="5" spans="2:16" ht="15.75" customHeight="1">
       <c r="F5" s="16"/>
@@ -1003,27 +1008,27 @@
       <c r="B9" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="57" t="s">
+      <c r="C9" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="57"/>
-      <c r="E9" s="57"/>
-      <c r="F9" s="58" t="s">
+      <c r="D9" s="56"/>
+      <c r="E9" s="56"/>
+      <c r="F9" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="G9" s="59"/>
-      <c r="H9" s="59"/>
-      <c r="I9" s="59"/>
-      <c r="J9" s="59"/>
-      <c r="K9" s="59"/>
-      <c r="L9" s="59"/>
+      <c r="G9" s="58"/>
+      <c r="H9" s="58"/>
+      <c r="I9" s="58"/>
+      <c r="J9" s="58"/>
+      <c r="K9" s="58"/>
+      <c r="L9" s="58"/>
       <c r="M9" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="N9" s="58" t="s">
+      <c r="N9" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="O9" s="66"/>
+      <c r="O9" s="59"/>
     </row>
     <row r="10" spans="2:16" ht="10.5" customHeight="1">
       <c r="B10" s="9"/>
@@ -1052,17 +1057,17 @@
       </c>
       <c r="F11" s="13"/>
       <c r="G11" s="29" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H11" s="29"/>
       <c r="I11" s="29"/>
       <c r="M11" s="10">
         <v>53.8</v>
       </c>
-      <c r="N11" s="62">
+      <c r="N11" s="60">
         <v>0.14899999999999999</v>
       </c>
-      <c r="O11" s="63"/>
+      <c r="O11" s="61"/>
     </row>
     <row r="12" spans="2:16" ht="15.75">
       <c r="B12" s="10"/>
@@ -1074,8 +1079,8 @@
       <c r="H12" s="29"/>
       <c r="I12" s="29"/>
       <c r="M12" s="10"/>
-      <c r="N12" s="62"/>
-      <c r="O12" s="63"/>
+      <c r="N12" s="60"/>
+      <c r="O12" s="61"/>
     </row>
     <row r="13" spans="2:16" ht="15.75">
       <c r="B13" s="10"/>
@@ -1087,8 +1092,8 @@
       <c r="H13" s="29"/>
       <c r="I13" s="29"/>
       <c r="M13" s="10"/>
-      <c r="N13" s="62"/>
-      <c r="O13" s="63"/>
+      <c r="N13" s="60"/>
+      <c r="O13" s="61"/>
     </row>
     <row r="14" spans="2:16" ht="15.75" customHeight="1">
       <c r="B14" s="10"/>
@@ -1096,8 +1101,8 @@
       <c r="E14" s="4"/>
       <c r="F14" s="3"/>
       <c r="M14" s="48"/>
-      <c r="N14" s="60"/>
-      <c r="O14" s="61"/>
+      <c r="N14" s="65"/>
+      <c r="O14" s="66"/>
     </row>
     <row r="15" spans="2:16" ht="9.75" customHeight="1">
       <c r="B15" s="32"/>
@@ -1260,7 +1265,7 @@
       </c>
       <c r="C30" s="15" t="str">
         <f>IF(ISBLANK(C2),"",C2)</f>
-        <v/>
+        <v>250215W99-WJY</v>
       </c>
       <c r="D30" s="15"/>
       <c r="E30" s="15"/>
@@ -1279,10 +1284,10 @@
       <c r="P30" s="54"/>
     </row>
     <row r="31" spans="2:16" ht="15.75" customHeight="1">
-      <c r="B31" s="56" t="s">
+      <c r="B31" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="C31" s="56"/>
+      <c r="C31" s="64"/>
       <c r="D31" s="53" t="str">
         <f>IF(ISBLANK(D3),"",D3)</f>
         <v/>
@@ -1350,7 +1355,7 @@
       </c>
       <c r="C35" s="53" t="str">
         <f>IF(ISBLANK(C7),"",C7)</f>
-        <v>W99-WJY-AIR</v>
+        <v>279-W99-WJY-AIR</v>
       </c>
       <c r="D35" s="15"/>
       <c r="E35" s="15"/>
@@ -1375,27 +1380,27 @@
       <c r="B37" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="C37" s="57" t="s">
+      <c r="C37" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="D37" s="57"/>
-      <c r="E37" s="57"/>
-      <c r="F37" s="58" t="s">
+      <c r="D37" s="56"/>
+      <c r="E37" s="56"/>
+      <c r="F37" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="G37" s="59"/>
-      <c r="H37" s="59"/>
-      <c r="I37" s="59"/>
-      <c r="J37" s="59"/>
-      <c r="K37" s="59"/>
-      <c r="L37" s="59"/>
+      <c r="G37" s="58"/>
+      <c r="H37" s="58"/>
+      <c r="I37" s="58"/>
+      <c r="J37" s="58"/>
+      <c r="K37" s="58"/>
+      <c r="L37" s="58"/>
       <c r="M37" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="N37" s="58" t="s">
+      <c r="N37" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="O37" s="66"/>
+      <c r="O37" s="59"/>
     </row>
     <row r="38" spans="2:16" ht="10.5" customHeight="1">
       <c r="B38" s="9"/>
@@ -1429,7 +1434,7 @@
       <c r="F39" s="13"/>
       <c r="G39" s="29" t="str">
         <f>IF(ISBLANK(G11),"",G11)</f>
-        <v>Aksesoris</v>
+        <v>A0034365  Aksesoris</v>
       </c>
       <c r="H39" s="29"/>
       <c r="I39" s="29"/>
@@ -1437,11 +1442,11 @@
         <f>IF(ISBLANK(M11),"",M11)</f>
         <v>53.8</v>
       </c>
-      <c r="N39" s="62">
+      <c r="N39" s="60">
         <f>IF(ISBLANK(N11),"",N11)</f>
         <v>0.14899999999999999</v>
       </c>
-      <c r="O39" s="63"/>
+      <c r="O39" s="61"/>
     </row>
     <row r="40" spans="2:16" ht="15.75">
       <c r="B40" s="10" t="str">
@@ -1465,11 +1470,11 @@
         <f>IF(ISBLANK(M12),"",M12)</f>
         <v/>
       </c>
-      <c r="N40" s="62" t="str">
+      <c r="N40" s="60" t="str">
         <f>IF(ISBLANK(N12),"",N12)</f>
         <v/>
       </c>
-      <c r="O40" s="63"/>
+      <c r="O40" s="61"/>
     </row>
     <row r="41" spans="2:16" ht="15.75">
       <c r="B41" s="10" t="str">
@@ -1493,11 +1498,11 @@
         <f t="shared" ref="M41:M42" si="4">IF(ISBLANK(M13),"",M13)</f>
         <v/>
       </c>
-      <c r="N41" s="62" t="str">
+      <c r="N41" s="60" t="str">
         <f t="shared" ref="N41:N42" si="5">IF(ISBLANK(N13),"",N13)</f>
         <v/>
       </c>
-      <c r="O41" s="63"/>
+      <c r="O41" s="61"/>
     </row>
     <row r="42" spans="2:16" ht="15.75" customHeight="1">
       <c r="B42" s="10" t="str">
@@ -1519,11 +1524,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="N42" s="62" t="str">
+      <c r="N42" s="60" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="O42" s="63"/>
+      <c r="O42" s="61"/>
     </row>
     <row r="43" spans="2:16" ht="9.75" customHeight="1">
       <c r="B43" s="48" t="str">
@@ -1666,22 +1671,6 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="M33:P33"/>
-    <mergeCell ref="M34:P34"/>
-    <mergeCell ref="M35:P35"/>
-    <mergeCell ref="C54:F54"/>
-    <mergeCell ref="C37:E37"/>
-    <mergeCell ref="F37:L37"/>
-    <mergeCell ref="N37:O37"/>
-    <mergeCell ref="N42:O42"/>
-    <mergeCell ref="N39:O39"/>
-    <mergeCell ref="N40:O40"/>
-    <mergeCell ref="N41:O41"/>
-    <mergeCell ref="M1:P1"/>
-    <mergeCell ref="M2:P2"/>
-    <mergeCell ref="M3:P3"/>
-    <mergeCell ref="M4:P4"/>
-    <mergeCell ref="N9:O9"/>
     <mergeCell ref="M32:P32"/>
     <mergeCell ref="C26:F26"/>
     <mergeCell ref="B3:C3"/>
@@ -1695,6 +1684,22 @@
     <mergeCell ref="N11:O11"/>
     <mergeCell ref="N12:O12"/>
     <mergeCell ref="N13:O13"/>
+    <mergeCell ref="M1:P1"/>
+    <mergeCell ref="M2:P2"/>
+    <mergeCell ref="M3:P3"/>
+    <mergeCell ref="M4:P4"/>
+    <mergeCell ref="N9:O9"/>
+    <mergeCell ref="M33:P33"/>
+    <mergeCell ref="M34:P34"/>
+    <mergeCell ref="M35:P35"/>
+    <mergeCell ref="C54:F54"/>
+    <mergeCell ref="C37:E37"/>
+    <mergeCell ref="F37:L37"/>
+    <mergeCell ref="N37:O37"/>
+    <mergeCell ref="N42:O42"/>
+    <mergeCell ref="N39:O39"/>
+    <mergeCell ref="N40:O40"/>
+    <mergeCell ref="N41:O41"/>
   </mergeCells>
   <pageMargins left="0.19685039370078741" right="0" top="0.23622047244094491" bottom="0.23622047244094491" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>